<commit_message>
Domino Pi rev. C: removed Schottky diode on +VUSB, it causes too much voltage drop, optimized power wiring, changed Logos
</commit_message>
<xml_diff>
--- a/Domino Pi/BOM/Domino Pi BOM.xlsx
+++ b/Domino Pi/BOM/Domino Pi BOM.xlsx
@@ -8,28 +8,29 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Pi Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Pi Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
   <si>
     <t>Item</t>
   </si>
@@ -58,18 +59,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>ACA-5036-A2-CC-S</t>
-  </si>
-  <si>
-    <t>INPAQ TECHNOLOGY</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>2.4GHZ CERAMIC CHIP ANTENNA</t>
-  </si>
-  <si>
     <t>1n</t>
   </si>
   <si>
@@ -214,60 +203,45 @@
     <t>CAP CER 4.7UF 6.3V 10% X5R 0402</t>
   </si>
   <si>
-    <t>MBRM130LT1G</t>
-  </si>
-  <si>
-    <t>ON SEMICONDUCTOR</t>
-  </si>
-  <si>
-    <t>DO-216AA</t>
+    <t>PRTR5V0U2X</t>
+  </si>
+  <si>
+    <t>NXP</t>
+  </si>
+  <si>
+    <t>SOT143B</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 30V 1A POWERMITE</t>
-  </si>
-  <si>
-    <t>PRTR5V0U2X</t>
-  </si>
-  <si>
-    <t>NXP</t>
-  </si>
-  <si>
-    <t>SOT143B</t>
+    <t>TVS DIODE ARRAY 2CH 5V SOT143</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>LED0603-RED</t>
+  </si>
+  <si>
+    <t>LED0603</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>TVS DIODE ARRAY 2CH 5V SOT143</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>LED0603-RED</t>
-  </si>
-  <si>
-    <t>LED0603</t>
+    <t>LED RED CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>LED0603-BLUE</t>
   </si>
   <si>
     <t>D3</t>
   </si>
   <si>
-    <t>LED RED CLEAR 0603 SMD</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>LED0603-BLUE</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>LED BLUE CLEAR 0603 SMD</t>
   </si>
   <si>
@@ -355,7 +329,7 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R1, R14</t>
+    <t>R1, R13</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -382,7 +356,7 @@
     <t>R0402_1k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R13</t>
+    <t>R14</t>
   </si>
   <si>
     <t>RES 1K OHM 1/16W 5% 0402 SMD</t>
@@ -454,22 +428,19 @@
     <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
   </si>
   <si>
-    <t>USB_MR5-003A</t>
+    <t>USB_MR5-001</t>
   </si>
   <si>
     <t>SZJUSTWELL ELECTRONICS</t>
   </si>
   <si>
-    <t>USB MR5-003A</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
     <t>CONN USB MICRO B RECPT SMT R/A</t>
   </si>
   <si>
-    <t>IT-1100</t>
+    <t>IT-1210</t>
   </si>
   <si>
     <t>SW1</t>
@@ -530,7 +501,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -558,6 +529,11 @@
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FFFFFF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -609,11 +585,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -631,22 +608,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.76470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.7058823529412"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.5607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.0509803921569"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.1843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.7921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8039215686274"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2078431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.356862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -692,16 +669,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
@@ -712,22 +689,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -735,25 +712,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -761,25 +738,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -787,25 +764,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -816,16 +793,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>35</v>
@@ -834,24 +811,24 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>39</v>
@@ -860,24 +837,24 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>43</v>
@@ -891,19 +868,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>47</v>
@@ -917,19 +894,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>51</v>
@@ -943,19 +920,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>55</v>
@@ -969,25 +946,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -998,22 +975,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -1024,16 +1001,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>69</v>
@@ -1053,10 +1030,10 @@
         <v>71</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>73</v>
@@ -1073,19 +1050,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>77</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>78</v>
@@ -1125,25 +1102,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
@@ -1154,48 +1131,48 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>91</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
+        <v>95</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
@@ -1206,42 +1183,42 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>102</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="23">
+        <v>105</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>108</v>
@@ -1261,22 +1238,22 @@
         <v>110</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>111</v>
       </c>
       <c r="F24" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="H24" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
@@ -1284,25 +1261,25 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="0" t="s">
+      <c r="H25" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="H25" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
@@ -1310,22 +1287,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="F26" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="0" t="s">
+      <c r="H26" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
@@ -1333,25 +1310,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="F27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="0" t="s">
+      <c r="H27" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
@@ -1362,48 +1339,48 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="H28" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
@@ -1413,49 +1390,49 @@
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>110</v>
+      <c r="C30" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>131</v>
+      <c r="C31" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
@@ -1466,22 +1443,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>141</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
@@ -1492,13 +1469,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>146</v>
@@ -1534,58 +1511,6 @@
       </c>
       <c r="H34" s="0" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="35">
-      <c r="A35" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="36">
-      <c r="A36" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Pi Rev. D: replaced resetable fuse by power swich, mino changes DC/DC layout and added more stitching vias
</commit_message>
<xml_diff>
--- a/Domino Pi/BOM/Domino Pi BOM.xlsx
+++ b/Domino Pi/BOM/Domino Pi BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Pi Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Pi Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. D'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="162">
   <si>
     <t>Item</t>
   </si>
@@ -59,54 +60,66 @@
     <t>Remarks</t>
   </si>
   <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>C0402_10n_X7R_10%_CER_50V</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C1, C20</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>C0402_1u_X7R_10%_CER_25V</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>22u</t>
+  </si>
+  <si>
+    <t>C0805_22u_X5R_20%_CER_6V3</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C14, C16</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 6.3V 20% X5R 0805</t>
+  </si>
+  <si>
     <t>1n</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>C1206_1n_X7R_10%_CER_500V</t>
   </si>
   <si>
     <t>C1206</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C2</t>
   </si>
   <si>
     <t>CAP CER 1000PF 500V 10% X7R 1206</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>C0402_1u_X7R_10%_CER_25V</t>
-  </si>
-  <si>
-    <t>C0402</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 25V 10% X7R 0402</t>
-  </si>
-  <si>
-    <t>22u</t>
-  </si>
-  <si>
-    <t>C0805_22u_X5R_20%_CER_6V3</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>C13, C15</t>
-  </si>
-  <si>
-    <t>CAP CER 22UF 6.3V 20% X5R 0805</t>
-  </si>
-  <si>
     <t>DNP</t>
   </si>
   <si>
@@ -116,7 +129,7 @@
     <t>C0402_DNP</t>
   </si>
   <si>
-    <t>C19(DNP), C21(DNP)</t>
+    <t>C21(DNP), C22(DNP)</t>
   </si>
   <si>
     <t>CAP DNP 0402</t>
@@ -125,79 +138,64 @@
     <t>C1206_22u_X7R_20%_CER_10V</t>
   </si>
   <si>
-    <t>C2</t>
+    <t>C3</t>
   </si>
   <si>
     <t>CAP CER 22UF 10V 20% X7R 1206</t>
   </si>
   <si>
-    <t>10n</t>
-  </si>
-  <si>
-    <t>C0402_10n_X7R_10%_CER_50V</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>CAP CER 10000PF 50V 10% X7R 0402</t>
-  </si>
-  <si>
     <t>10p</t>
   </si>
   <si>
     <t>C0402_10p_NP0_5%_CER_50V</t>
   </si>
   <si>
-    <t>C3, C16</t>
+    <t>C4, C17</t>
   </si>
   <si>
     <t>CAP CER 10PF 50V 5% NP0 0402</t>
   </si>
   <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>C0805_10u_X5R_10%_CER_16V</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 16V 10% X5R 0805</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
     <t>C0402_100n_X7R_10%_CER_50V</t>
   </si>
   <si>
-    <t>C5, C6, C9, C10, C12, C14, C17</t>
+    <t>C5, C6, C10, C11, C13, C15, C18</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
   </si>
   <si>
+    <t>4u7</t>
+  </si>
+  <si>
+    <t>C0805_4u7_X5R_10%_CER_16V</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V 10% X5R 0805</t>
+  </si>
+  <si>
     <t>22p</t>
   </si>
   <si>
     <t>C0402_22p_NP0_5%_CER_50V</t>
   </si>
   <si>
-    <t>C7</t>
+    <t>C8</t>
   </si>
   <si>
     <t>CAP CER 22PF 50V 5% NP0 0402</t>
   </si>
   <si>
-    <t>4u7</t>
-  </si>
-  <si>
     <t>C0402_4u7_X5R_10%_CER_6V3</t>
   </si>
   <si>
-    <t>C8, C18</t>
+    <t>C9, C19</t>
   </si>
   <si>
     <t>CAP CER 4.7UF 6.3V 10% X5R 0402</t>
@@ -221,43 +219,28 @@
     <t>RED</t>
   </si>
   <si>
-    <t>LED0603-RED</t>
-  </si>
-  <si>
-    <t>LED0603</t>
+    <t>LED0402-RED</t>
+  </si>
+  <si>
+    <t>LED0402</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>LED RED CLEAR 0603 SMD</t>
+    <t>LED RED CLEAR 0402 SMD</t>
   </si>
   <si>
     <t>BLUE</t>
   </si>
   <si>
-    <t>LED0603-BLUE</t>
+    <t>LED0402-BLUE</t>
   </si>
   <si>
     <t>D3</t>
   </si>
   <si>
-    <t>LED BLUE CLEAR 0603 SMD</t>
-  </si>
-  <si>
-    <t>0ZCG0110FF2C</t>
-  </si>
-  <si>
-    <t>BEL FUSE INC</t>
-  </si>
-  <si>
-    <t>PTC1812</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>PTC RESETTBLE 1.10A 8V CHIP 1812</t>
+    <t>LED BLUE CLEAR 0402 SMD</t>
   </si>
   <si>
     <t>MH28-1</t>
@@ -329,7 +312,7 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R1, R13</t>
+    <t>R1, R15</t>
   </si>
   <si>
     <t>RES 10K OHM 1/16W 5% 0402 SMD</t>
@@ -338,13 +321,34 @@
     <t>270R</t>
   </si>
   <si>
+    <t>R0402_270R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>RES 270 OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R0603_0R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
+  </si>
+  <si>
     <t>R0603_270R_5%_125mW</t>
   </si>
   <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>R10</t>
+    <t>R13</t>
   </si>
   <si>
     <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
@@ -356,7 +360,7 @@
     <t>R0402_1k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R14</t>
+    <t>R17</t>
   </si>
   <si>
     <t>RES 1K OHM 1/16W 5% 0402 SMD</t>
@@ -374,66 +378,75 @@
     <t>RES 33.2K OHM 1/16W 1% 0402 SMD</t>
   </si>
   <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R0402_100k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
     <t>150k</t>
   </si>
   <si>
     <t>R0402_150k_1%_62.5mW</t>
   </si>
   <si>
-    <t>R3</t>
+    <t>R4</t>
   </si>
   <si>
     <t>RES 150K OHM 1/16W 1% 0402 SMD</t>
   </si>
   <si>
+    <t>R0402_0R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R5, R9, R10, R14, R16</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>R0402_15k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>RES 15K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
     <t>47k</t>
   </si>
   <si>
     <t>R0402_47k_5%_62.5mW</t>
   </si>
   <si>
-    <t>R4, R5(DNP)</t>
+    <t>R7, R8(DNP)</t>
   </si>
   <si>
     <t>RES 47K OHM 1/16W 5% 0402 SMD</t>
   </si>
   <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>R0402_0R_5%_62.5mW</t>
-  </si>
-  <si>
-    <t>R6, R7, R11, R12</t>
-  </si>
-  <si>
-    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
-  </si>
-  <si>
-    <t>R0402_270R_5%_62.5mW</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>RES 270 OHM 1/16W 5% 0402 SMD</t>
-  </si>
-  <si>
-    <t>R0603_0R_5%_125mW</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>RES 0.0 OHM 1/8W JUMP SMD 0603</t>
-  </si>
-  <si>
     <t>USB_MR5-001</t>
   </si>
   <si>
     <t>SZJUSTWELL ELECTRONICS</t>
   </si>
   <si>
+    <t>USB MR5-001</t>
+  </si>
+  <si>
+    <t>USB-MR5-001</t>
+  </si>
+  <si>
     <t>S1</t>
   </si>
   <si>
@@ -449,16 +462,28 @@
     <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
   </si>
   <si>
+    <t>MP65151DJ</t>
+  </si>
+  <si>
+    <t>MONOLITHIC POWER</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC POWER SWITCH 1.7A SOT23-6</t>
+  </si>
+  <si>
     <t>MP2162GQH</t>
   </si>
   <si>
-    <t>MONOLITHIC POWER</t>
-  </si>
-  <si>
     <t>QFN-8_2X1.5</t>
   </si>
   <si>
-    <t>U1</t>
+    <t>U2</t>
   </si>
   <si>
     <t>IC REG BUCK SYNC ADJ 2A 8WDFN</t>
@@ -473,7 +498,7 @@
     <t>QFN-25_4X4</t>
   </si>
   <si>
-    <t>U2</t>
+    <t>U3</t>
   </si>
   <si>
     <t>IC SGL USB-TO-UART BRIDGE 24QFN</t>
@@ -488,7 +513,7 @@
     <t>SC70</t>
   </si>
   <si>
-    <t>U3</t>
+    <t>U4</t>
   </si>
   <si>
     <t>IC BUFF/DVR TRI-ST N-INV SC705</t>
@@ -501,7 +526,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -529,11 +554,6 @@
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FFFFFF"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -585,12 +605,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -608,22 +627,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
+      <selection activeCell="E19" activeCellId="0" pane="topLeft" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8039215686274"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.356862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -660,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -698,13 +717,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -715,22 +734,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -738,25 +757,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -764,25 +783,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -793,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
@@ -802,7 +821,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>35</v>
@@ -828,7 +847,7 @@
         <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>39</v>
@@ -842,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>41</v>
@@ -854,7 +873,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>43</v>
@@ -868,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>45</v>
@@ -880,7 +899,7 @@
         <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>47</v>
@@ -906,7 +925,7 @@
         <v>50</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>51</v>
@@ -923,22 +942,22 @@
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
@@ -949,22 +968,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -975,22 +994,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -1001,22 +1020,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
@@ -1024,25 +1043,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -1050,25 +1069,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -1079,13 +1098,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>82</v>
@@ -1114,13 +1133,13 @@
         <v>87</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
@@ -1128,25 +1147,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="G20" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="0" t="s">
+      <c r="H20" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="21">
@@ -1154,25 +1173,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
@@ -1183,22 +1202,22 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
@@ -1209,22 +1228,22 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
@@ -1235,22 +1254,22 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
@@ -1261,22 +1280,22 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="26">
@@ -1287,22 +1306,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
@@ -1310,25 +1329,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
@@ -1336,25 +1355,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
@@ -1365,22 +1384,22 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
@@ -1390,23 +1409,23 @@
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="H30" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
@@ -1416,23 +1435,23 @@
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>136</v>
+      <c r="F31" s="0" t="s">
+        <v>137</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
@@ -1443,22 +1462,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="F32" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
@@ -1469,22 +1488,22 @@
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="G33" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="H33" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="34">
@@ -1495,22 +1514,74 @@
         <v>1</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="G34" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="H34" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G34" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>153</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domnio Pi Rev. E: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino Pi/BOM/Domino Pi BOM.xlsx
+++ b/Domino Pi/BOM/Domino Pi BOM.xlsx
@@ -8,23 +8,24 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="114" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Pi Rev. D" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Pi Rev. E" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. D'!$A$2:$I$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Pi Rev. E'!$A$2:$I$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Pi Rev. E'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -634,15 +635,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6392156862745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2980392156863"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -1532,7 +1533,7 @@
         <v>151</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>

</xml_diff>